<commit_message>
mettre à jour l'exercice
</commit_message>
<xml_diff>
--- a/luxstrat/excel/Exercice_1_énoncé.xlsx
+++ b/luxstrat/excel/Exercice_1_énoncé.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Nextcloud\io-footprinting\luxstrat\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64921912-BB8C-4EB0-BA01-11C8BE572565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868796C1-9C03-4A51-9FFC-104494D5F2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9C020466-51D9-4448-9A5B-695F5741AD9C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{9C020466-51D9-4448-9A5B-695F5741AD9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercice 1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,6 @@
     <sheet name="Exercice 3" sheetId="4" r:id="rId3"/>
     <sheet name="bridge 3-to-7" sheetId="3" r:id="rId4"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
     <definedName name="GHG">'Exercice 2'!$M$6:$M$8</definedName>
   </definedNames>
@@ -45,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1338,7 +1335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1545,10 +1542,22 @@
     <xf numFmtId="1" fontId="2" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1558,6 +1567,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1572,34 +1584,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7731,139 +7727,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Exercice 1"/>
-      <sheetName val="Exercice 2"/>
-      <sheetName val="Exercice 3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="130">
-          <cell r="B130" t="str">
-            <v>I*y</v>
-          </cell>
-          <cell r="C130" t="str">
-            <v>(I+A)*y</v>
-          </cell>
-          <cell r="D130" t="str">
-            <v>(I+A+A2)*y</v>
-          </cell>
-          <cell r="E130" t="str">
-            <v>(I+A+A2+A3)*y</v>
-          </cell>
-          <cell r="F130" t="str">
-            <v>(I+A+A2+A3+A4)*y</v>
-          </cell>
-          <cell r="G130" t="str">
-            <v>(I+A+A2+A3+A4+A5)*y</v>
-          </cell>
-        </row>
-        <row r="131">
-          <cell r="A131" t="str">
-            <v>Ag-&gt;MC</v>
-          </cell>
-          <cell r="B131">
-            <v>0</v>
-          </cell>
-          <cell r="C131">
-            <v>13.248071216617211</v>
-          </cell>
-          <cell r="D131">
-            <v>17.978153991860058</v>
-          </cell>
-          <cell r="E131">
-            <v>19.573614612543654</v>
-          </cell>
-          <cell r="F131">
-            <v>20.143113158448518</v>
-          </cell>
-          <cell r="G131">
-            <v>20.356568237978447</v>
-          </cell>
-        </row>
-        <row r="132">
-          <cell r="A132" t="str">
-            <v>MC-&gt;MC</v>
-          </cell>
-          <cell r="B132">
-            <v>1063</v>
-          </cell>
-          <cell r="C132">
-            <v>1360.1353115727004</v>
-          </cell>
-          <cell r="D132">
-            <v>1457.2445021997407</v>
-          </cell>
-          <cell r="E132">
-            <v>1492.0587941939282</v>
-          </cell>
-          <cell r="F132">
-            <v>1505.1900790485809</v>
-          </cell>
-          <cell r="G132">
-            <v>1510.2736144778835</v>
-          </cell>
-        </row>
-        <row r="133">
-          <cell r="A133" t="str">
-            <v>Se-&gt;MC</v>
-          </cell>
-          <cell r="B133">
-            <v>0</v>
-          </cell>
-          <cell r="C133">
-            <v>212.60000000000002</v>
-          </cell>
-          <cell r="D133">
-            <v>337.42148633518218</v>
-          </cell>
-          <cell r="E133">
-            <v>394.5118886272578</v>
-          </cell>
-          <cell r="F133">
-            <v>418.56822898147107</v>
-          </cell>
-          <cell r="G133">
-            <v>428.37274097073521</v>
-          </cell>
-        </row>
-        <row r="134">
-          <cell r="A134" t="str">
-            <v>Se-Se</v>
-          </cell>
-          <cell r="B134">
-            <v>1518</v>
-          </cell>
-          <cell r="C134">
-            <v>1962.4050056882822</v>
-          </cell>
-          <cell r="D134">
-            <v>2109.1084159889201</v>
-          </cell>
-          <cell r="E134">
-            <v>2161.7948549949651</v>
-          </cell>
-          <cell r="F134">
-            <v>2181.6714989395955</v>
-          </cell>
-          <cell r="G134">
-            <v>2189.3663213241925</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8163,7 +8026,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0258745-312D-430B-ADDC-6FE62853A492}">
   <dimension ref="A1:AD134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView topLeftCell="A115" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F140" sqref="F140"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8276,63 +8141,63 @@
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="195" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="195"/>
-      <c r="D22" s="195"/>
-      <c r="E22" s="195" t="s">
+      <c r="B22" s="198" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="198"/>
+      <c r="D22" s="198"/>
+      <c r="E22" s="198" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="195"/>
-      <c r="G22" s="195"/>
-      <c r="H22" s="195"/>
-      <c r="I22" s="195"/>
+      <c r="F22" s="198"/>
+      <c r="G22" s="198"/>
+      <c r="H22" s="198"/>
+      <c r="I22" s="198"/>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="186" t="s">
+      <c r="B23" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="189" t="s">
+      <c r="C23" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="186" t="s">
+      <c r="D23" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="186" t="s">
+      <c r="E23" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="186"/>
-      <c r="G23" s="186" t="s">
+      <c r="F23" s="199"/>
+      <c r="G23" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="186" t="s">
+      <c r="H23" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="I23" s="186" t="s">
+      <c r="I23" s="199" t="s">
         <v>8</v>
       </c>
-      <c r="J23" s="186" t="s">
+      <c r="J23" s="199" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="188"/>
-      <c r="C24" s="190"/>
-      <c r="D24" s="188"/>
+      <c r="B24" s="200"/>
+      <c r="C24" s="202"/>
+      <c r="D24" s="200"/>
       <c r="E24" s="24" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G24" s="186"/>
-      <c r="H24" s="186"/>
-      <c r="I24" s="186"/>
-      <c r="J24" s="187"/>
+      <c r="G24" s="199"/>
+      <c r="H24" s="199"/>
+      <c r="I24" s="199"/>
+      <c r="J24" s="203"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
@@ -8742,20 +8607,20 @@
       <c r="A47" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="191" t="s">
+      <c r="B47" s="204" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="193" t="s">
+      <c r="C47" s="206" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="191" t="s">
+      <c r="D47" s="204" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B48" s="192"/>
-      <c r="C48" s="194"/>
-      <c r="D48" s="192"/>
+      <c r="B48" s="205"/>
+      <c r="C48" s="207"/>
+      <c r="D48" s="205"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
@@ -8881,20 +8746,20 @@
       <c r="A69" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B69" s="186" t="s">
+      <c r="B69" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="189" t="s">
+      <c r="C69" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="D69" s="186" t="s">
+      <c r="D69" s="199" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B70" s="188"/>
-      <c r="C70" s="190"/>
-      <c r="D70" s="188"/>
+      <c r="B70" s="200"/>
+      <c r="C70" s="202"/>
+      <c r="D70" s="200"/>
       <c r="G70" s="4" t="s">
         <v>43</v>
       </c>
@@ -8979,20 +8844,20 @@
       <c r="A83" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B83" s="186" t="s">
+      <c r="B83" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C83" s="189" t="s">
+      <c r="C83" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="D83" s="186" t="s">
+      <c r="D83" s="199" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B84" s="188"/>
-      <c r="C84" s="190"/>
-      <c r="D84" s="188"/>
+      <c r="B84" s="200"/>
+      <c r="C84" s="202"/>
+      <c r="D84" s="200"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
@@ -9060,7 +8925,7 @@
         <f>SUM(E25:I25)</f>
         <v>17</v>
       </c>
-      <c r="E95" s="209"/>
+      <c r="E95" s="195"/>
       <c r="G95" s="61">
         <f t="array" ref="G95:G97">J25:J27</f>
         <v>0</v>
@@ -9083,12 +8948,12 @@
         <f t="shared" ref="B96:B97" si="5">SUM(E26:I26)</f>
         <v>1063</v>
       </c>
-      <c r="E96" s="210"/>
+      <c r="E96" s="196"/>
       <c r="G96" s="62">
         <v>0</v>
       </c>
       <c r="I96" s="36"/>
-      <c r="J96" s="212"/>
+      <c r="J96" s="37"/>
       <c r="K96" s="182"/>
     </row>
     <row r="97" spans="1:27" x14ac:dyDescent="0.2">
@@ -9099,7 +8964,7 @@
         <f t="shared" si="5"/>
         <v>1518</v>
       </c>
-      <c r="E97" s="211"/>
+      <c r="E97" s="197"/>
       <c r="G97" s="63">
         <v>0</v>
       </c>
@@ -9766,12 +9631,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:F23"/>
     <mergeCell ref="J23:J24"/>
     <mergeCell ref="B69:B70"/>
     <mergeCell ref="C69:C70"/>
@@ -9785,6 +9644,12 @@
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:F23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{EF3F5A55-55C8-40CA-BE00-39AA66C5486B}"/>
@@ -9820,16 +9685,16 @@
       <c r="D3" s="69"/>
       <c r="E3" s="69"/>
       <c r="F3" s="69"/>
-      <c r="L3" s="197" t="s">
+      <c r="L3" s="210" t="s">
         <v>79</v>
       </c>
-      <c r="M3" s="197"/>
-      <c r="N3" s="197"/>
+      <c r="M3" s="210"/>
+      <c r="N3" s="210"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="L4" s="197"/>
-      <c r="M4" s="197"/>
-      <c r="N4" s="197"/>
+      <c r="L4" s="210"/>
+      <c r="M4" s="210"/>
+      <c r="N4" s="210"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
@@ -9858,19 +9723,19 @@
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="195" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="195"/>
-      <c r="D7" s="195"/>
-      <c r="E7" s="195" t="s">
+      <c r="B7" s="198" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="198"/>
+      <c r="D7" s="198"/>
+      <c r="E7" s="198" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="195"/>
-      <c r="G7" s="195"/>
-      <c r="H7" s="195"/>
-      <c r="I7" s="195"/>
-      <c r="J7" s="186" t="s">
+      <c r="F7" s="198"/>
+      <c r="G7" s="198"/>
+      <c r="H7" s="198"/>
+      <c r="I7" s="198"/>
+      <c r="J7" s="199" t="s">
         <v>2</v>
       </c>
       <c r="L7" s="72" t="s">
@@ -9887,29 +9752,29 @@
       <c r="A8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="186" t="s">
+      <c r="B8" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="189" t="s">
+      <c r="C8" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="186" t="s">
+      <c r="D8" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="196" t="s">
+      <c r="E8" s="208" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="196"/>
-      <c r="G8" s="186" t="s">
+      <c r="F8" s="208"/>
+      <c r="G8" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="186" t="s">
+      <c r="H8" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="186" t="s">
+      <c r="I8" s="199" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="186"/>
+      <c r="J8" s="199"/>
       <c r="L8" s="72" t="s">
         <v>63</v>
       </c>
@@ -9922,19 +9787,19 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="188"/>
-      <c r="C9" s="190"/>
-      <c r="D9" s="188"/>
+      <c r="B9" s="200"/>
+      <c r="C9" s="202"/>
+      <c r="D9" s="200"/>
       <c r="E9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="186"/>
-      <c r="H9" s="186"/>
-      <c r="I9" s="186"/>
-      <c r="J9" s="186"/>
+      <c r="G9" s="199"/>
+      <c r="H9" s="199"/>
+      <c r="I9" s="199"/>
+      <c r="J9" s="199"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -9963,12 +9828,12 @@
       <c r="K10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L10" s="198" t="s">
+      <c r="L10" s="209" t="s">
         <v>66</v>
       </c>
-      <c r="M10" s="198"/>
-      <c r="N10" s="198"/>
-      <c r="O10" s="198"/>
+      <c r="M10" s="209"/>
+      <c r="N10" s="209"/>
+      <c r="O10" s="209"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -9997,10 +9862,10 @@
       <c r="K11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L11" s="198"/>
-      <c r="M11" s="198"/>
-      <c r="N11" s="198"/>
-      <c r="O11" s="198"/>
+      <c r="L11" s="209"/>
+      <c r="M11" s="209"/>
+      <c r="N11" s="209"/>
+      <c r="O11" s="209"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
@@ -10029,10 +9894,10 @@
       <c r="K12" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L12" s="198"/>
-      <c r="M12" s="198"/>
-      <c r="N12" s="198"/>
-      <c r="O12" s="198"/>
+      <c r="L12" s="209"/>
+      <c r="M12" s="209"/>
+      <c r="N12" s="209"/>
+      <c r="O12" s="209"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
@@ -10077,19 +9942,19 @@
       <c r="A20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="195" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="195"/>
-      <c r="D20" s="195"/>
-      <c r="E20" s="195" t="s">
+      <c r="B20" s="198" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="198"/>
+      <c r="D20" s="198"/>
+      <c r="E20" s="198" t="s">
         <v>1</v>
       </c>
-      <c r="F20" s="195"/>
-      <c r="G20" s="195"/>
-      <c r="H20" s="195"/>
-      <c r="I20" s="195"/>
-      <c r="J20" s="186" t="s">
+      <c r="F20" s="198"/>
+      <c r="G20" s="198"/>
+      <c r="H20" s="198"/>
+      <c r="I20" s="198"/>
+      <c r="J20" s="199" t="s">
         <v>2</v>
       </c>
     </row>
@@ -10097,45 +9962,45 @@
       <c r="A21" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="186" t="s">
+      <c r="B21" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="189" t="s">
+      <c r="C21" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="186" t="s">
+      <c r="D21" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="196" t="s">
+      <c r="E21" s="208" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="196"/>
-      <c r="G21" s="186" t="s">
+      <c r="F21" s="208"/>
+      <c r="G21" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="186" t="s">
+      <c r="H21" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="186" t="s">
+      <c r="I21" s="199" t="s">
         <v>8</v>
       </c>
-      <c r="J21" s="186"/>
+      <c r="J21" s="199"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="188"/>
-      <c r="C22" s="190"/>
-      <c r="D22" s="188"/>
+      <c r="B22" s="200"/>
+      <c r="C22" s="202"/>
+      <c r="D22" s="200"/>
       <c r="E22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="186"/>
-      <c r="H22" s="186"/>
-      <c r="I22" s="186"/>
-      <c r="J22" s="186"/>
+      <c r="G22" s="199"/>
+      <c r="H22" s="199"/>
+      <c r="I22" s="199"/>
+      <c r="J22" s="199"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
@@ -10231,19 +10096,19 @@
       <c r="A32" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="195" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="195"/>
-      <c r="D32" s="195"/>
-      <c r="E32" s="195" t="s">
+      <c r="B32" s="198" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="198"/>
+      <c r="D32" s="198"/>
+      <c r="E32" s="198" t="s">
         <v>1</v>
       </c>
-      <c r="F32" s="195"/>
-      <c r="G32" s="195"/>
-      <c r="H32" s="195"/>
-      <c r="I32" s="195"/>
-      <c r="J32" s="186" t="s">
+      <c r="F32" s="198"/>
+      <c r="G32" s="198"/>
+      <c r="H32" s="198"/>
+      <c r="I32" s="198"/>
+      <c r="J32" s="199" t="s">
         <v>2</v>
       </c>
     </row>
@@ -10251,45 +10116,45 @@
       <c r="A33" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="186" t="s">
+      <c r="B33" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="189" t="s">
+      <c r="C33" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="186" t="s">
+      <c r="D33" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="E33" s="196" t="s">
+      <c r="E33" s="208" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="196"/>
-      <c r="G33" s="186" t="s">
+      <c r="F33" s="208"/>
+      <c r="G33" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="186" t="s">
+      <c r="H33" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="I33" s="186" t="s">
+      <c r="I33" s="199" t="s">
         <v>8</v>
       </c>
-      <c r="J33" s="186"/>
+      <c r="J33" s="199"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
-      <c r="B34" s="188"/>
-      <c r="C34" s="190"/>
-      <c r="D34" s="188"/>
+      <c r="B34" s="200"/>
+      <c r="C34" s="202"/>
+      <c r="D34" s="200"/>
       <c r="E34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G34" s="186"/>
-      <c r="H34" s="186"/>
-      <c r="I34" s="186"/>
-      <c r="J34" s="186"/>
+      <c r="G34" s="199"/>
+      <c r="H34" s="199"/>
+      <c r="I34" s="199"/>
+      <c r="J34" s="199"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
@@ -10383,19 +10248,19 @@
       <c r="A44" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="195" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="195"/>
-      <c r="D44" s="195"/>
-      <c r="E44" s="195" t="s">
+      <c r="B44" s="198" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="198"/>
+      <c r="D44" s="198"/>
+      <c r="E44" s="198" t="s">
         <v>1</v>
       </c>
-      <c r="F44" s="195"/>
-      <c r="G44" s="195"/>
-      <c r="H44" s="195"/>
-      <c r="I44" s="195"/>
-      <c r="J44" s="186" t="s">
+      <c r="F44" s="198"/>
+      <c r="G44" s="198"/>
+      <c r="H44" s="198"/>
+      <c r="I44" s="198"/>
+      <c r="J44" s="199" t="s">
         <v>2</v>
       </c>
     </row>
@@ -10403,45 +10268,45 @@
       <c r="A45" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="186" t="s">
+      <c r="B45" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="189" t="s">
+      <c r="C45" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="186" t="s">
+      <c r="D45" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="196" t="s">
+      <c r="E45" s="208" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="196"/>
-      <c r="G45" s="186" t="s">
+      <c r="F45" s="208"/>
+      <c r="G45" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="H45" s="186" t="s">
+      <c r="H45" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="I45" s="186" t="s">
+      <c r="I45" s="199" t="s">
         <v>8</v>
       </c>
-      <c r="J45" s="186"/>
+      <c r="J45" s="199"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
-      <c r="B46" s="188"/>
-      <c r="C46" s="190"/>
-      <c r="D46" s="188"/>
+      <c r="B46" s="200"/>
+      <c r="C46" s="202"/>
+      <c r="D46" s="200"/>
       <c r="E46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G46" s="186"/>
-      <c r="H46" s="186"/>
-      <c r="I46" s="186"/>
-      <c r="J46" s="186"/>
+      <c r="G46" s="199"/>
+      <c r="H46" s="199"/>
+      <c r="I46" s="199"/>
+      <c r="J46" s="199"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
@@ -10532,17 +10397,17 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B57" s="196" t="s">
+      <c r="B57" s="208" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="196"/>
-      <c r="D57" s="186" t="s">
+      <c r="C57" s="208"/>
+      <c r="D57" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="186" t="s">
+      <c r="E57" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="F57" s="186" t="s">
+      <c r="F57" s="199" t="s">
         <v>8</v>
       </c>
     </row>
@@ -10553,9 +10418,9 @@
       <c r="C58" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D58" s="186"/>
-      <c r="E58" s="186"/>
-      <c r="F58" s="186"/>
+      <c r="D58" s="199"/>
+      <c r="E58" s="199"/>
+      <c r="F58" s="199"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
@@ -10614,30 +10479,11 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="L10:O12"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="J44:J46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="E45:F45"/>
     <mergeCell ref="L3:N4"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="E32:I32"/>
@@ -10650,16 +10496,35 @@
     <mergeCell ref="H33:H34"/>
     <mergeCell ref="I33:I34"/>
     <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="J44:J46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
     <mergeCell ref="G45:G46"/>
     <mergeCell ref="H45:H46"/>
     <mergeCell ref="I45:I46"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="E44:I44"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="L10:O12"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10670,7 +10535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FA19E7-3E6D-4DFA-B17B-2674996F2278}">
   <dimension ref="A1:W141"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28:Q33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10695,102 +10562,102 @@
       </c>
     </row>
     <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="195" t="s">
+      <c r="C4" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="195"/>
-      <c r="E4" s="195"/>
-      <c r="F4" s="195" t="s">
+      <c r="D4" s="198"/>
+      <c r="E4" s="198"/>
+      <c r="F4" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="G4" s="195"/>
-      <c r="H4" s="195"/>
-      <c r="I4" s="195" t="s">
+      <c r="G4" s="198"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="J4" s="195"/>
-      <c r="K4" s="195"/>
-      <c r="L4" s="195"/>
-      <c r="M4" s="195" t="s">
+      <c r="J4" s="198"/>
+      <c r="K4" s="198"/>
+      <c r="L4" s="198"/>
+      <c r="M4" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="N4" s="195"/>
-      <c r="O4" s="195"/>
-      <c r="P4" s="195"/>
+      <c r="N4" s="198"/>
+      <c r="O4" s="198"/>
+      <c r="P4" s="198"/>
     </row>
     <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="B5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="186" t="s">
+      <c r="C5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="189" t="s">
+      <c r="D5" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="186" t="s">
+      <c r="E5" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="186" t="s">
+      <c r="F5" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="189" t="s">
+      <c r="G5" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="186" t="s">
+      <c r="H5" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="186" t="s">
+      <c r="I5" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="186"/>
-      <c r="K5" s="186" t="s">
+      <c r="J5" s="199"/>
+      <c r="K5" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="186" t="s">
+      <c r="L5" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="186" t="s">
+      <c r="M5" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="186"/>
-      <c r="O5" s="186" t="s">
+      <c r="N5" s="199"/>
+      <c r="O5" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="P5" s="186" t="s">
+      <c r="P5" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="186" t="s">
+      <c r="Q5" s="199" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="23.25" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="188"/>
-      <c r="D6" s="190"/>
-      <c r="E6" s="188"/>
-      <c r="F6" s="188"/>
-      <c r="G6" s="190"/>
-      <c r="H6" s="188"/>
+      <c r="C6" s="200"/>
+      <c r="D6" s="202"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="200"/>
+      <c r="G6" s="202"/>
+      <c r="H6" s="200"/>
       <c r="I6" s="24" t="s">
         <v>9</v>
       </c>
       <c r="J6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="186"/>
-      <c r="L6" s="186"/>
+      <c r="K6" s="199"/>
+      <c r="L6" s="199"/>
       <c r="M6" s="24" t="s">
         <v>9</v>
       </c>
       <c r="N6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="186"/>
-      <c r="P6" s="186"/>
-      <c r="Q6" s="187"/>
+      <c r="O6" s="199"/>
+      <c r="P6" s="199"/>
+      <c r="Q6" s="203"/>
     </row>
     <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="199" t="s">
+      <c r="A7" s="211" t="s">
         <v>93</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -10844,7 +10711,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="199"/>
+      <c r="A8" s="211"/>
       <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
@@ -10896,7 +10763,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="199"/>
+      <c r="A9" s="211"/>
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
@@ -10948,7 +10815,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="199" t="s">
+      <c r="A10" s="211" t="s">
         <v>94</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -10965,15 +10832,15 @@
       </c>
       <c r="F10" s="11">
         <f ca="1">RANDBETWEEN(50,150)/100/0.043*C7</f>
-        <v>102.33964685920463</v>
+        <v>36.897967915223447</v>
       </c>
       <c r="G10" s="11">
         <f t="shared" ref="G10:H10" ca="1" si="1">RANDBETWEEN(50,150)/100/0.043*D7</f>
-        <v>462.80135007165211</v>
+        <v>537.44672911546695</v>
       </c>
       <c r="H10" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>24.969383076759268</v>
+        <v>34.770449331188132</v>
       </c>
       <c r="I10" s="4">
         <v>8</v>
@@ -10989,7 +10856,7 @@
       </c>
       <c r="M10" s="11">
         <f t="shared" ref="M10:P12" ca="1" si="2">RANDBETWEEN(50,150)/100/0.043*I7</f>
-        <v>198.83720930232559</v>
+        <v>263.72093023255815</v>
       </c>
       <c r="N10" s="11">
         <f t="shared" ca="1" si="2"/>
@@ -11001,15 +10868,15 @@
       </c>
       <c r="P10" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>53.720930232558146</v>
+        <v>44.651162790697683</v>
       </c>
       <c r="Q10" s="39">
         <f t="shared" ca="1" si="0"/>
-        <v>896.66851954249978</v>
+        <v>971.48723938513433</v>
       </c>
     </row>
     <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="199"/>
+      <c r="A11" s="211"/>
       <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
@@ -11024,7 +10891,7 @@
       </c>
       <c r="F11" s="11">
         <f t="shared" ref="F11:F12" ca="1" si="3">RANDBETWEEN(50,150)/100/0.043*C8</f>
-        <v>206.49263041480651</v>
+        <v>132.22773702000768</v>
       </c>
       <c r="G11" s="11">
         <f t="shared" ref="G11:G12" ca="1" si="4">RANDBETWEEN(50,150)/100/0.043*D8</f>
@@ -11032,7 +10899,7 @@
       </c>
       <c r="H11" s="11">
         <f t="shared" ref="H11:H12" ca="1" si="5">RANDBETWEEN(50,150)/100/0.043*E8</f>
-        <v>3946.2932881839743</v>
+        <v>3714.1583888790356</v>
       </c>
       <c r="I11" s="4">
         <v>20</v>
@@ -11048,27 +10915,27 @@
       </c>
       <c r="M11" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>8895.3488372093034</v>
+        <v>8480.2325581395344</v>
       </c>
       <c r="N11" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>151.39534883720933</v>
+        <v>224.65116279069767</v>
       </c>
       <c r="O11" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>7901.3953488372099</v>
+        <v>6574.8837209302328</v>
       </c>
       <c r="P11" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>-1213.953488372093</v>
+        <v>-1564.6511627906978</v>
       </c>
       <c r="Q11" s="39">
         <f t="shared" ca="1" si="0"/>
-        <v>32835.860152624198</v>
+        <v>30510.390592482599</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="12" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="199"/>
+      <c r="A12" s="211"/>
       <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
@@ -11083,15 +10950,15 @@
       </c>
       <c r="F12" s="11">
         <f t="shared" ca="1" si="3"/>
-        <v>288.84212628626915</v>
+        <v>136.46084706437912</v>
       </c>
       <c r="G12" s="11">
         <f t="shared" ca="1" si="4"/>
-        <v>4000.7827769691548</v>
+        <v>8707.5860439916905</v>
       </c>
       <c r="H12" s="11">
         <f t="shared" ca="1" si="5"/>
-        <v>26570.067370679375</v>
+        <v>24415.737583867536</v>
       </c>
       <c r="I12" s="4">
         <v>100</v>
@@ -11107,23 +10974,23 @@
       </c>
       <c r="M12" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>13010.232558139536</v>
+        <v>19876.744186046515</v>
       </c>
       <c r="N12" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>13674.418604651162</v>
+        <v>17093.023255813958</v>
       </c>
       <c r="O12" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>828.83720930232562</v>
+        <v>1949.3023255813955</v>
       </c>
       <c r="P12" s="11">
         <f t="shared" ca="1" si="2"/>
-        <v>173.02325581395348</v>
+        <v>182.79069767441862</v>
       </c>
       <c r="Q12" s="40">
         <f t="shared" ca="1" si="0"/>
-        <v>58783.203901841778</v>
+        <v>72598.644940039885</v>
       </c>
     </row>
     <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
@@ -11144,15 +11011,15 @@
       </c>
       <c r="F13" s="15">
         <f t="shared" ca="1" si="6"/>
-        <v>621.67440356028033</v>
+        <v>329.58655199961026</v>
       </c>
       <c r="G13" s="15">
         <f t="shared" ca="1" si="6"/>
-        <v>17230.472314554594</v>
+        <v>22011.920960620944</v>
       </c>
       <c r="H13" s="15">
         <f t="shared" ca="1" si="6"/>
-        <v>31091.330041940109</v>
+        <v>28714.66642207776</v>
       </c>
       <c r="I13" s="16">
         <f t="shared" si="6"/>
@@ -11176,7 +11043,7 @@
       <c r="P13" s="95"/>
       <c r="Q13" s="32">
         <f ca="1">SUM(C13:L13)</f>
-        <v>53156.303520005975</v>
+        <v>55269.000694649309</v>
       </c>
     </row>
     <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
@@ -11217,15 +11084,15 @@
       </c>
       <c r="F15" s="11">
         <f ca="1">RANDBETWEEN(50,150)/100/0.043*C15</f>
-        <v>57.209302325581397</v>
+        <v>26.976744186046513</v>
       </c>
       <c r="G15" s="29">
         <f t="shared" ref="G15:H15" ca="1" si="7">RANDBETWEEN(50,150)/100/0.043*D15</f>
-        <v>242.7906976744186</v>
+        <v>184.18604651162792</v>
       </c>
       <c r="H15" s="29">
         <f t="shared" ca="1" si="7"/>
-        <v>1047.6744186046512</v>
+        <v>1035.3488372093022</v>
       </c>
       <c r="I15" s="4">
         <v>151</v>
@@ -11238,7 +11105,7 @@
       </c>
       <c r="Q15" s="9">
         <f ca="1">SUM(C15:L15)</f>
-        <v>1605.6744186046512</v>
+        <v>1504.5116279069766</v>
       </c>
     </row>
     <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
@@ -11259,15 +11126,15 @@
       </c>
       <c r="F16" s="15">
         <f t="shared" ca="1" si="8"/>
-        <v>678.88370588586167</v>
+        <v>356.56329618565678</v>
       </c>
       <c r="G16" s="15">
         <f t="shared" ca="1" si="8"/>
-        <v>17473.263012229014</v>
+        <v>22196.107007132574</v>
       </c>
       <c r="H16" s="15">
         <f t="shared" ca="1" si="8"/>
-        <v>32139.004460544762</v>
+        <v>29750.015259287062</v>
       </c>
       <c r="I16" s="16">
         <f t="shared" si="8"/>
@@ -11291,7 +11158,7 @@
       <c r="P16" s="16"/>
       <c r="Q16" s="15">
         <f ca="1">SUM(Q13:Q15)</f>
-        <v>54761.977938610624</v>
+        <v>56773.512322556286</v>
       </c>
     </row>
     <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
@@ -11309,19 +11176,19 @@
       </c>
       <c r="F17" s="29">
         <f ca="1">RANDBETWEEN(50,100)/100/0.043*C17</f>
-        <v>115.17585674441385</v>
+        <v>119.05818899422556</v>
       </c>
       <c r="G17" s="29">
         <f t="shared" ref="G17:H20" ca="1" si="9">RANDBETWEEN(50,100)/100/0.043*D17</f>
-        <v>4555.731720707272</v>
+        <v>5782.2748762823066</v>
       </c>
       <c r="H17" s="29">
         <f t="shared" ca="1" si="9"/>
-        <v>19343.438507252369</v>
+        <v>12435.067611805096</v>
       </c>
       <c r="Q17" s="15">
         <f ca="1">SUM(C17:L17)</f>
-        <v>25245.37744015321</v>
+        <v>19567.432032530785</v>
       </c>
     </row>
     <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
@@ -11339,19 +11206,19 @@
       </c>
       <c r="F18" s="29">
         <f t="shared" ref="F18:F20" ca="1" si="10">RANDBETWEEN(50,100)/100/0.043*C18</f>
-        <v>-86.511627906976742</v>
+        <v>-96.279069767441854</v>
       </c>
       <c r="G18" s="29">
         <f t="shared" ca="1" si="9"/>
-        <v>-38.604651162790702</v>
+        <v>-34.883720930232563</v>
       </c>
       <c r="H18" s="29">
         <f t="shared" ca="1" si="9"/>
-        <v>-51.627906976744192</v>
+        <v>-64.186046511627922</v>
       </c>
       <c r="Q18" s="15">
         <f ca="1">SUM(C18:L18)</f>
-        <v>-187.74418604651163</v>
+        <v>-206.34883720930233</v>
       </c>
     </row>
     <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
@@ -11369,19 +11236,19 @@
       </c>
       <c r="F19" s="29">
         <f t="shared" ca="1" si="10"/>
-        <v>146.97674418604652</v>
+        <v>148.83720930232559</v>
       </c>
       <c r="G19" s="29">
         <f t="shared" ca="1" si="9"/>
-        <v>1719.0697674418604</v>
+        <v>1093.9534883720933</v>
       </c>
       <c r="H19" s="29">
         <f t="shared" ca="1" si="9"/>
-        <v>5067.6744186046517</v>
+        <v>3948.8372093023254</v>
       </c>
       <c r="Q19" s="15">
         <f ca="1">SUM(C19:L19)</f>
-        <v>7308.7209302325591</v>
+        <v>5566.6279069767443</v>
       </c>
     </row>
     <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
@@ -11399,19 +11266,19 @@
       </c>
       <c r="F20" s="29">
         <f t="shared" ca="1" si="10"/>
-        <v>84.651162790697683</v>
+        <v>151.39534883720933</v>
       </c>
       <c r="G20" s="29">
         <f t="shared" ca="1" si="9"/>
-        <v>1344.1860465116281</v>
+        <v>1897.6744186046512</v>
       </c>
       <c r="H20" s="29">
         <f t="shared" ca="1" si="9"/>
-        <v>8400</v>
+        <v>9200.0000000000018</v>
       </c>
       <c r="Q20" s="15">
         <f ca="1">SUM(C20:L20)</f>
-        <v>10350.837209302326</v>
+        <v>11771.069767441862</v>
       </c>
     </row>
     <row r="21" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
@@ -11432,15 +11299,15 @@
       </c>
       <c r="F21" s="31">
         <f t="shared" ca="1" si="11"/>
-        <v>260.29213581418134</v>
+        <v>323.01167736631862</v>
       </c>
       <c r="G21" s="31">
         <f t="shared" ca="1" si="11"/>
-        <v>7580.3828834979695</v>
+        <v>8739.0190623288181</v>
       </c>
       <c r="H21" s="31">
         <f t="shared" ca="1" si="11"/>
-        <v>32759.485018880277</v>
+        <v>25519.718774595793</v>
       </c>
       <c r="I21" s="20"/>
       <c r="J21" s="20"/>
@@ -11452,7 +11319,7 @@
       <c r="P21" s="96"/>
       <c r="Q21" s="15">
         <f ca="1">SUM(C21:L21)</f>
-        <v>42717.19139364158</v>
+        <v>36698.780869740083</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="12" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -11473,15 +11340,15 @@
       </c>
       <c r="F22" s="42">
         <f t="shared" ca="1" si="12"/>
-        <v>939.17584170004307</v>
+        <v>679.5749735519754</v>
       </c>
       <c r="G22" s="42">
         <f t="shared" ca="1" si="12"/>
-        <v>25053.645895726982</v>
+        <v>30935.126069461392</v>
       </c>
       <c r="H22" s="43">
         <f t="shared" ca="1" si="12"/>
-        <v>64898.489479425043</v>
+        <v>55269.734033882851</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" ref="I22:L22" si="13">SUM(I16+I21)</f>
@@ -11509,106 +11376,106 @@
     </row>
     <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C25" s="195" t="s">
+      <c r="C25" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="D25" s="195"/>
-      <c r="E25" s="195"/>
-      <c r="F25" s="195" t="s">
+      <c r="D25" s="198"/>
+      <c r="E25" s="198"/>
+      <c r="F25" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="G25" s="195"/>
-      <c r="H25" s="195"/>
-      <c r="I25" s="195" t="s">
+      <c r="G25" s="198"/>
+      <c r="H25" s="198"/>
+      <c r="I25" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="J25" s="195"/>
-      <c r="K25" s="195"/>
-      <c r="L25" s="195"/>
-      <c r="M25" s="195" t="s">
+      <c r="J25" s="198"/>
+      <c r="K25" s="198"/>
+      <c r="L25" s="198"/>
+      <c r="M25" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="N25" s="195"/>
-      <c r="O25" s="195"/>
-      <c r="P25" s="195"/>
+      <c r="N25" s="198"/>
+      <c r="O25" s="198"/>
+      <c r="P25" s="198"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B26" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="186" t="s">
+      <c r="C26" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="189" t="s">
+      <c r="D26" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="186" t="s">
+      <c r="E26" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="186" t="s">
+      <c r="F26" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="189" t="s">
+      <c r="G26" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="H26" s="186" t="s">
+      <c r="H26" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="186" t="s">
+      <c r="I26" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="J26" s="186"/>
-      <c r="K26" s="186" t="s">
+      <c r="J26" s="199"/>
+      <c r="K26" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="L26" s="186" t="s">
+      <c r="L26" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="M26" s="186" t="s">
+      <c r="M26" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="N26" s="186"/>
-      <c r="O26" s="186" t="s">
+      <c r="N26" s="199"/>
+      <c r="O26" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="P26" s="186" t="s">
+      <c r="P26" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="Q26" s="186" t="s">
+      <c r="Q26" s="199" t="s">
         <v>2</v>
       </c>
-      <c r="S26" s="186" t="s">
+      <c r="S26" s="199" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="186"/>
-      <c r="D27" s="189"/>
-      <c r="E27" s="186"/>
-      <c r="F27" s="186"/>
-      <c r="G27" s="189"/>
-      <c r="H27" s="186"/>
+      <c r="C27" s="199"/>
+      <c r="D27" s="201"/>
+      <c r="E27" s="199"/>
+      <c r="F27" s="199"/>
+      <c r="G27" s="201"/>
+      <c r="H27" s="199"/>
       <c r="I27" s="24" t="s">
         <v>9</v>
       </c>
       <c r="J27" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K27" s="186"/>
-      <c r="L27" s="186"/>
+      <c r="K27" s="199"/>
+      <c r="L27" s="199"/>
       <c r="M27" s="24" t="s">
         <v>9</v>
       </c>
       <c r="N27" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O27" s="186"/>
-      <c r="P27" s="186"/>
-      <c r="Q27" s="187"/>
-      <c r="S27" s="186"/>
+      <c r="O27" s="199"/>
+      <c r="P27" s="199"/>
+      <c r="Q27" s="203"/>
+      <c r="S27" s="199"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A28" s="199" t="s">
+      <c r="A28" s="211" t="s">
         <v>93</v>
       </c>
       <c r="B28" s="4" t="s">
@@ -11656,17 +11523,14 @@
       <c r="P28" s="8">
         <v>0</v>
       </c>
-      <c r="Q28" s="99">
-        <f t="shared" ref="Q28:Q33" si="14">SUM(C28:P28)</f>
-        <v>42.395393207687704</v>
-      </c>
+      <c r="Q28" s="99"/>
       <c r="S28" s="141">
-        <f t="shared" ref="S28:S33" si="15">SUM(I28:P28)</f>
+        <f t="shared" ref="S28:S33" si="14">SUM(I28:P28)</f>
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A29" s="199"/>
+      <c r="A29" s="211"/>
       <c r="B29" s="4" t="s">
         <v>21</v>
       </c>
@@ -11712,17 +11576,14 @@
       <c r="P29" s="12">
         <v>0</v>
       </c>
-      <c r="Q29" s="97">
+      <c r="Q29" s="97"/>
+      <c r="S29" s="142">
         <f t="shared" si="14"/>
-        <v>1685.3625982928302</v>
-      </c>
-      <c r="S29" s="142">
-        <f t="shared" si="15"/>
         <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A30" s="199"/>
+      <c r="A30" s="211"/>
       <c r="B30" s="4" t="s">
         <v>22</v>
       </c>
@@ -11768,17 +11629,14 @@
       <c r="P30" s="12">
         <v>0</v>
       </c>
-      <c r="Q30" s="97">
+      <c r="Q30" s="97"/>
+      <c r="S30" s="142">
         <f t="shared" si="14"/>
-        <v>2637.0687684504719</v>
-      </c>
-      <c r="S30" s="142">
-        <f t="shared" si="15"/>
         <v>1349</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A31" s="199" t="s">
+      <c r="A31" s="211" t="s">
         <v>94</v>
       </c>
       <c r="B31" s="4" t="s">
@@ -11826,17 +11684,14 @@
       <c r="P31" s="103">
         <v>44.651162790697683</v>
       </c>
-      <c r="Q31" s="97">
+      <c r="Q31" s="97"/>
+      <c r="S31" s="142">
         <f t="shared" si="14"/>
-        <v>930.20630434794191</v>
-      </c>
-      <c r="S31" s="142">
-        <f t="shared" si="15"/>
         <v>193.6511627906977</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A32" s="199"/>
+      <c r="A32" s="211"/>
       <c r="B32" s="4" t="s">
         <v>21</v>
       </c>
@@ -11882,17 +11737,14 @@
       <c r="P32" s="103">
         <v>-1820.9302325581398</v>
       </c>
-      <c r="Q32" s="97">
+      <c r="Q32" s="97"/>
+      <c r="S32" s="142">
         <f t="shared" si="14"/>
-        <v>26533.17232500458</v>
-      </c>
-      <c r="S32" s="142">
-        <f t="shared" si="15"/>
         <v>7685.0232558139542</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="199"/>
+      <c r="A33" s="211"/>
       <c r="B33" s="4" t="s">
         <v>22</v>
       </c>
@@ -11931,7 +11783,7 @@
       </c>
       <c r="N33" s="11">
         <f>10027.9069767442+H42-46166</f>
-        <v>9851.7134683236509</v>
+        <v>-36138.093023255802</v>
       </c>
       <c r="O33" s="11">
         <v>1504.1860465116281</v>
@@ -11939,13 +11791,10 @@
       <c r="P33" s="103">
         <v>99.069767441860478</v>
       </c>
-      <c r="Q33" s="100">
+      <c r="Q33" s="100"/>
+      <c r="S33" s="143">
         <f t="shared" si="14"/>
-        <v>45989.980425546964</v>
-      </c>
-      <c r="S33" s="143">
-        <f t="shared" si="15"/>
-        <v>21147.946026463185</v>
+        <v>-24841.860465116268</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
@@ -11957,55 +11806,55 @@
         <v>25.56205986940148</v>
       </c>
       <c r="D34" s="15">
-        <f t="shared" ref="D34" si="16">SUM(D28:D33)</f>
+        <f t="shared" ref="D34" si="15">SUM(D28:D33)</f>
         <v>1129.6959315463573</v>
       </c>
       <c r="E34" s="15">
-        <f t="shared" ref="E34" si="17">SUM(E28:E33)</f>
+        <f t="shared" ref="E34" si="16">SUM(E28:E33)</f>
         <v>1025.5687685352309</v>
       </c>
       <c r="F34" s="15">
-        <f t="shared" ref="F34" si="18">SUM(F28:F33)</f>
+        <f t="shared" ref="F34" si="17">SUM(F28:F33)</f>
         <v>620.46126090635721</v>
       </c>
       <c r="G34" s="15">
-        <f t="shared" ref="G34" si="19">SUM(G28:G33)</f>
+        <f t="shared" ref="G34" si="18">SUM(G28:G33)</f>
         <v>21762.548880742284</v>
       </c>
       <c r="H34" s="15">
-        <f t="shared" ref="H34" si="20">SUM(H28:H33)</f>
+        <f t="shared" ref="H34" si="19">SUM(H28:H33)</f>
         <v>22373.728468183013</v>
       </c>
       <c r="I34" s="16">
-        <f t="shared" ref="I34" si="21">SUM(I28:I33)</f>
+        <f t="shared" ref="I34" si="20">SUM(I28:I33)</f>
         <v>1169</v>
       </c>
       <c r="J34" s="16">
-        <f t="shared" ref="J34" si="22">SUM(J28:J33)</f>
+        <f t="shared" ref="J34" si="21">SUM(J28:J33)</f>
         <v>506</v>
       </c>
       <c r="K34" s="16">
-        <f t="shared" ref="K34" si="23">SUM(K28:K33)</f>
+        <f t="shared" ref="K34" si="22">SUM(K28:K33)</f>
         <v>375</v>
       </c>
       <c r="L34" s="15">
-        <f t="shared" ref="L34" si="24">SUM(L28:L33)</f>
+        <f t="shared" ref="L34" si="23">SUM(L28:L33)</f>
         <v>-18</v>
       </c>
       <c r="M34" s="32">
-        <f t="shared" ref="M34" si="25">SUM(M28:M33)</f>
+        <f t="shared" ref="M34" si="24">SUM(M28:M33)</f>
         <v>15982.720930232561</v>
       </c>
       <c r="N34" s="32">
-        <f t="shared" ref="N34" si="26">SUM(N28:N33)</f>
-        <v>10038.922770649233</v>
+        <f t="shared" ref="N34" si="25">SUM(N28:N33)</f>
+        <v>-35950.883720930222</v>
       </c>
       <c r="O34" s="32">
-        <f t="shared" ref="O34" si="27">SUM(O28:O33)</f>
+        <f t="shared" ref="O34" si="26">SUM(O28:O33)</f>
         <v>4504.1860465116279</v>
       </c>
       <c r="P34" s="104">
-        <f t="shared" ref="P34" si="28">SUM(P28:P33)</f>
+        <f t="shared" ref="P34" si="27">SUM(P28:P33)</f>
         <v>-1677.2093023255816</v>
       </c>
       <c r="Q34" s="32">
@@ -12064,59 +11913,59 @@
         <v>14</v>
       </c>
       <c r="C36" s="14">
-        <f t="shared" ref="C36:L36" si="29">SUM(C34:C35)</f>
+        <f t="shared" ref="C36:L36" si="28">SUM(C34:C35)</f>
         <v>27.56205986940148</v>
       </c>
       <c r="D36" s="15">
+        <f t="shared" si="28"/>
+        <v>1141.6959315463573</v>
+      </c>
+      <c r="E36" s="15">
+        <f t="shared" si="28"/>
+        <v>1078.5687685352309</v>
+      </c>
+      <c r="F36" s="15">
+        <f t="shared" si="28"/>
+        <v>683.25195858077586</v>
+      </c>
+      <c r="G36" s="15">
+        <f t="shared" si="28"/>
+        <v>21960.688415626006</v>
+      </c>
+      <c r="H36" s="15">
+        <f t="shared" si="28"/>
+        <v>23125.588933299292</v>
+      </c>
+      <c r="I36" s="16">
+        <f t="shared" si="28"/>
+        <v>1320</v>
+      </c>
+      <c r="J36" s="16">
+        <f t="shared" si="28"/>
+        <v>512</v>
+      </c>
+      <c r="K36" s="16">
+        <f t="shared" si="28"/>
+        <v>409</v>
+      </c>
+      <c r="L36" s="15">
+        <f t="shared" si="28"/>
+        <v>-18</v>
+      </c>
+      <c r="M36" s="15">
+        <f t="shared" ref="M36:P36" si="29">SUM(M34:M35)</f>
+        <v>18482.720930232561</v>
+      </c>
+      <c r="N36" s="15">
         <f t="shared" si="29"/>
-        <v>1141.6959315463573</v>
-      </c>
-      <c r="E36" s="15">
+        <v>-35860.883720930222</v>
+      </c>
+      <c r="O36" s="15">
         <f t="shared" si="29"/>
-        <v>1078.5687685352309</v>
-      </c>
-      <c r="F36" s="15">
+        <v>5004.1860465116279</v>
+      </c>
+      <c r="P36" s="105">
         <f t="shared" si="29"/>
-        <v>683.25195858077586</v>
-      </c>
-      <c r="G36" s="15">
-        <f t="shared" si="29"/>
-        <v>21960.688415626006</v>
-      </c>
-      <c r="H36" s="15">
-        <f t="shared" si="29"/>
-        <v>23125.588933299292</v>
-      </c>
-      <c r="I36" s="16">
-        <f t="shared" si="29"/>
-        <v>1320</v>
-      </c>
-      <c r="J36" s="16">
-        <f t="shared" si="29"/>
-        <v>512</v>
-      </c>
-      <c r="K36" s="16">
-        <f t="shared" si="29"/>
-        <v>409</v>
-      </c>
-      <c r="L36" s="15">
-        <f t="shared" si="29"/>
-        <v>-18</v>
-      </c>
-      <c r="M36" s="15">
-        <f t="shared" ref="M36:P36" si="30">SUM(M34:M35)</f>
-        <v>18482.720930232561</v>
-      </c>
-      <c r="N36" s="15">
-        <f t="shared" si="30"/>
-        <v>10128.922770649233</v>
-      </c>
-      <c r="O36" s="15">
-        <f t="shared" si="30"/>
-        <v>5004.1860465116279</v>
-      </c>
-      <c r="P36" s="105">
-        <f t="shared" si="30"/>
         <v>-1677.2093023255816</v>
       </c>
       <c r="Q36" s="15">
@@ -12142,7 +11991,7 @@
       </c>
       <c r="G37" s="29">
         <f>5694.66465088409+Q32-30728</f>
-        <v>1499.8369758886693</v>
+        <v>-25033.335349115911</v>
       </c>
       <c r="H37" s="29">
         <v>9869.1012792103938</v>
@@ -12150,7 +11999,7 @@
       <c r="P37" s="12"/>
       <c r="Q37" s="15">
         <f>SUM(C37:L37)</f>
-        <v>12677.616255544453</v>
+        <v>-13855.556069460126</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
@@ -12246,23 +12095,23 @@
         <v>14.564676224730107</v>
       </c>
       <c r="D41" s="27">
-        <f t="shared" ref="D41:H41" si="31">SUM(D37:D40)</f>
+        <f t="shared" ref="D41:H41" si="30">SUM(D37:D40)</f>
         <v>543.72396921233212</v>
       </c>
       <c r="E41" s="27">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>1558.7427100120938</v>
       </c>
       <c r="F41" s="27">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>246.94897057762944</v>
       </c>
       <c r="G41" s="27">
-        <f t="shared" si="31"/>
-        <v>4572.3951154235538</v>
+        <f t="shared" si="30"/>
+        <v>-21960.777209581025</v>
       </c>
       <c r="H41" s="27">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>22864.217558280161</v>
       </c>
       <c r="I41" s="20"/>
@@ -12275,166 +12124,148 @@
       <c r="P41" s="21"/>
       <c r="Q41" s="15">
         <f>SUM(C41:L41)</f>
-        <v>29800.592999730499</v>
+        <v>3267.4206747259195</v>
       </c>
     </row>
     <row r="42" spans="1:19" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="101">
-        <f>C36+C41</f>
-        <v>42.126736094131587</v>
-      </c>
-      <c r="D42" s="102">
-        <f t="shared" ref="D42" si="32">D36+D41</f>
-        <v>1685.4199007586894</v>
-      </c>
-      <c r="E42" s="102">
-        <f t="shared" ref="E42" si="33">E36+E41</f>
-        <v>2637.3114785473244</v>
-      </c>
-      <c r="F42" s="102">
-        <f t="shared" ref="F42" si="34">F36+F41</f>
-        <v>930.2009291584053</v>
-      </c>
-      <c r="G42" s="102">
-        <f t="shared" ref="G42" si="35">G36+G41</f>
-        <v>26533.08353104956</v>
-      </c>
-      <c r="H42" s="100">
-        <f t="shared" ref="H42" si="36">H36+H41</f>
-        <v>45989.806491579453</v>
-      </c>
+      <c r="C42" s="101"/>
+      <c r="D42" s="102"/>
+      <c r="E42" s="102"/>
+      <c r="F42" s="102"/>
+      <c r="G42" s="102"/>
+      <c r="H42" s="100"/>
       <c r="I42" s="1">
-        <f t="shared" ref="I42:P42" si="37">SUM(I36+I41)</f>
+        <f t="shared" ref="I42:P42" si="31">SUM(I36+I41)</f>
         <v>1320</v>
       </c>
       <c r="J42" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>512</v>
       </c>
       <c r="K42" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>409</v>
       </c>
       <c r="L42" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>-18</v>
       </c>
       <c r="M42" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>18482.720930232561</v>
       </c>
       <c r="N42" s="9">
-        <f t="shared" si="37"/>
-        <v>10128.922770649233</v>
+        <f t="shared" si="31"/>
+        <v>-35860.883720930222</v>
       </c>
       <c r="O42" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>5004.1860465116279</v>
       </c>
       <c r="P42" s="9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="31"/>
         <v>-1677.2093023255816</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="C47" s="195" t="s">
+      <c r="C47" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="D47" s="195"/>
-      <c r="E47" s="195"/>
-      <c r="F47" s="195" t="s">
+      <c r="D47" s="198"/>
+      <c r="E47" s="198"/>
+      <c r="F47" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="G47" s="195"/>
-      <c r="H47" s="195"/>
-      <c r="I47" s="195" t="s">
+      <c r="G47" s="198"/>
+      <c r="H47" s="198"/>
+      <c r="I47" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="J47" s="195"/>
-      <c r="K47" s="195"/>
-      <c r="L47" s="195"/>
-      <c r="M47" s="195" t="s">
+      <c r="J47" s="198"/>
+      <c r="K47" s="198"/>
+      <c r="L47" s="198"/>
+      <c r="M47" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="N47" s="195"/>
-      <c r="O47" s="195"/>
-      <c r="P47" s="195"/>
+      <c r="N47" s="198"/>
+      <c r="O47" s="198"/>
+      <c r="P47" s="198"/>
     </row>
     <row r="48" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="186" t="s">
+      <c r="C48" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="189" t="s">
+      <c r="D48" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="186" t="s">
+      <c r="E48" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="186" t="s">
+      <c r="F48" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="G48" s="189" t="s">
+      <c r="G48" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="H48" s="186" t="s">
+      <c r="H48" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="I48" s="186" t="s">
+      <c r="I48" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="J48" s="186"/>
-      <c r="K48" s="186" t="s">
+      <c r="J48" s="199"/>
+      <c r="K48" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="L48" s="186" t="s">
+      <c r="L48" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="M48" s="186" t="s">
+      <c r="M48" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="N48" s="186"/>
-      <c r="O48" s="186" t="s">
+      <c r="N48" s="199"/>
+      <c r="O48" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="P48" s="186" t="s">
+      <c r="P48" s="199" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:23" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="C49" s="186"/>
-      <c r="D49" s="189"/>
-      <c r="E49" s="186"/>
-      <c r="F49" s="186"/>
-      <c r="G49" s="189"/>
-      <c r="H49" s="186"/>
+      <c r="C49" s="199"/>
+      <c r="D49" s="201"/>
+      <c r="E49" s="199"/>
+      <c r="F49" s="199"/>
+      <c r="G49" s="201"/>
+      <c r="H49" s="199"/>
       <c r="I49" s="24" t="s">
         <v>9</v>
       </c>
       <c r="J49" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K49" s="186"/>
-      <c r="L49" s="186"/>
+      <c r="K49" s="199"/>
+      <c r="L49" s="199"/>
       <c r="M49" s="24" t="s">
         <v>9</v>
       </c>
       <c r="N49" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O49" s="186"/>
-      <c r="P49" s="186"/>
+      <c r="O49" s="199"/>
+      <c r="P49" s="199"/>
       <c r="R49" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A50" s="199" t="s">
+      <c r="A50" s="211" t="s">
         <v>93</v>
       </c>
       <c r="B50" s="4" t="s">
@@ -12474,7 +12305,7 @@
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A51" s="199"/>
+      <c r="A51" s="211"/>
       <c r="B51" s="4" t="s">
         <v>21</v>
       </c>
@@ -12505,7 +12336,7 @@
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A52" s="199"/>
+      <c r="A52" s="211"/>
       <c r="B52" s="4" t="s">
         <v>22</v>
       </c>
@@ -12536,7 +12367,7 @@
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A53" s="199" t="s">
+      <c r="A53" s="211" t="s">
         <v>94</v>
       </c>
       <c r="B53" s="4" t="s">
@@ -12572,7 +12403,7 @@
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A54" s="199"/>
+      <c r="A54" s="211"/>
       <c r="B54" s="4" t="s">
         <v>21</v>
       </c>
@@ -12606,7 +12437,7 @@
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A55" s="199"/>
+      <c r="A55" s="211"/>
       <c r="B55" s="4" t="s">
         <v>22</v>
       </c>
@@ -12765,23 +12596,23 @@
         <v>0</v>
       </c>
       <c r="D64" s="121">
-        <f t="shared" ref="D64" si="38">D58+D63</f>
+        <f t="shared" ref="D64" si="32">D58+D63</f>
         <v>0</v>
       </c>
       <c r="E64" s="121">
-        <f t="shared" ref="E64" si="39">E58+E63</f>
+        <f t="shared" ref="E64" si="33">E58+E63</f>
         <v>0</v>
       </c>
       <c r="F64" s="121">
-        <f t="shared" ref="F64" si="40">F58+F63</f>
+        <f t="shared" ref="F64" si="34">F58+F63</f>
         <v>0</v>
       </c>
       <c r="G64" s="121">
-        <f t="shared" ref="G64" si="41">G58+G63</f>
+        <f t="shared" ref="G64" si="35">G58+G63</f>
         <v>0</v>
       </c>
       <c r="H64" s="122">
-        <f t="shared" ref="H64" si="42">H58+H63</f>
+        <f t="shared" ref="H64" si="36">H58+H63</f>
         <v>0</v>
       </c>
       <c r="I64" s="1"/>
@@ -12794,50 +12625,50 @@
       <c r="P64" s="9"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C67" s="195" t="s">
+      <c r="C67" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="D67" s="195"/>
-      <c r="E67" s="195"/>
-      <c r="F67" s="195" t="s">
+      <c r="D67" s="198"/>
+      <c r="E67" s="198"/>
+      <c r="F67" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="195"/>
-      <c r="H67" s="195"/>
+      <c r="G67" s="198"/>
+      <c r="H67" s="198"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B68" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C68" s="186" t="s">
+      <c r="C68" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="D68" s="189" t="s">
+      <c r="D68" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="E68" s="186" t="s">
+      <c r="E68" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="F68" s="186" t="s">
+      <c r="F68" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="G68" s="189" t="s">
+      <c r="G68" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="H68" s="186" t="s">
+      <c r="H68" s="199" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C69" s="186"/>
-      <c r="D69" s="189"/>
-      <c r="E69" s="186"/>
-      <c r="F69" s="186"/>
-      <c r="G69" s="189"/>
-      <c r="H69" s="186"/>
+      <c r="C69" s="199"/>
+      <c r="D69" s="201"/>
+      <c r="E69" s="199"/>
+      <c r="F69" s="199"/>
+      <c r="G69" s="201"/>
+      <c r="H69" s="199"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="199" t="s">
+      <c r="A70" s="211" t="s">
         <v>93</v>
       </c>
       <c r="B70" s="4" t="s">
@@ -12864,7 +12695,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="199"/>
+      <c r="A71" s="211"/>
       <c r="B71" s="4" t="s">
         <v>21</v>
       </c>
@@ -12888,7 +12719,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="199"/>
+      <c r="A72" s="211"/>
       <c r="B72" s="4" t="s">
         <v>22</v>
       </c>
@@ -12912,7 +12743,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="199" t="s">
+      <c r="A73" s="211" t="s">
         <v>94</v>
       </c>
       <c r="B73" s="4" t="s">
@@ -12938,7 +12769,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="199"/>
+      <c r="A74" s="211"/>
       <c r="B74" s="4" t="s">
         <v>21</v>
       </c>
@@ -12962,7 +12793,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="199"/>
+      <c r="A75" s="211"/>
       <c r="B75" s="4" t="s">
         <v>22</v>
       </c>
@@ -12986,50 +12817,50 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C78" s="195" t="s">
+      <c r="C78" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="D78" s="195"/>
-      <c r="E78" s="195"/>
-      <c r="F78" s="195" t="s">
+      <c r="D78" s="198"/>
+      <c r="E78" s="198"/>
+      <c r="F78" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="G78" s="195"/>
-      <c r="H78" s="195"/>
+      <c r="G78" s="198"/>
+      <c r="H78" s="198"/>
     </row>
     <row r="79" spans="1:8" ht="12" x14ac:dyDescent="0.2">
       <c r="B79" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C79" s="186" t="s">
+      <c r="C79" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="D79" s="189" t="s">
+      <c r="D79" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="E79" s="186" t="s">
+      <c r="E79" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="F79" s="186" t="s">
+      <c r="F79" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="G79" s="189" t="s">
+      <c r="G79" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="H79" s="186" t="s">
+      <c r="H79" s="199" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C80" s="186"/>
-      <c r="D80" s="189"/>
-      <c r="E80" s="186"/>
-      <c r="F80" s="186"/>
-      <c r="G80" s="189"/>
-      <c r="H80" s="186"/>
+      <c r="C80" s="199"/>
+      <c r="D80" s="201"/>
+      <c r="E80" s="199"/>
+      <c r="F80" s="199"/>
+      <c r="G80" s="201"/>
+      <c r="H80" s="199"/>
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A81" s="199" t="s">
+      <c r="A81" s="211" t="s">
         <v>93</v>
       </c>
       <c r="B81" s="4" t="s">
@@ -13056,7 +12887,7 @@
       </c>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A82" s="199"/>
+      <c r="A82" s="211"/>
       <c r="B82" s="4" t="s">
         <v>21</v>
       </c>
@@ -13080,7 +12911,7 @@
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A83" s="199"/>
+      <c r="A83" s="211"/>
       <c r="B83" s="4" t="s">
         <v>22</v>
       </c>
@@ -13104,7 +12935,7 @@
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A84" s="199" t="s">
+      <c r="A84" s="211" t="s">
         <v>94</v>
       </c>
       <c r="B84" s="4" t="s">
@@ -13130,7 +12961,7 @@
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A85" s="199"/>
+      <c r="A85" s="211"/>
       <c r="B85" s="4" t="s">
         <v>21</v>
       </c>
@@ -13154,7 +12985,7 @@
       </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A86" s="199"/>
+      <c r="A86" s="211"/>
       <c r="B86" s="4" t="s">
         <v>22</v>
       </c>
@@ -13181,29 +13012,29 @@
       <c r="B90" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C90" s="195" t="s">
+      <c r="C90" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="D90" s="195"/>
-      <c r="E90" s="195"/>
-      <c r="F90" s="195" t="s">
+      <c r="D90" s="198"/>
+      <c r="E90" s="198"/>
+      <c r="F90" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="G90" s="195"/>
-      <c r="H90" s="195"/>
-      <c r="I90" s="195" t="s">
+      <c r="G90" s="198"/>
+      <c r="H90" s="198"/>
+      <c r="I90" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="J90" s="195"/>
-      <c r="K90" s="195"/>
-      <c r="L90" s="195"/>
-      <c r="M90" s="195" t="s">
+      <c r="J90" s="198"/>
+      <c r="K90" s="198"/>
+      <c r="L90" s="198"/>
+      <c r="M90" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="N90" s="195"/>
-      <c r="O90" s="195"/>
-      <c r="P90" s="195"/>
-      <c r="Q90" s="186" t="s">
+      <c r="N90" s="198"/>
+      <c r="O90" s="198"/>
+      <c r="P90" s="198"/>
+      <c r="Q90" s="199" t="s">
         <v>52</v>
       </c>
     </row>
@@ -13211,70 +13042,70 @@
       <c r="B91" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C91" s="186" t="s">
+      <c r="C91" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="D91" s="189" t="s">
+      <c r="D91" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="E91" s="186" t="s">
+      <c r="E91" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="F91" s="186" t="s">
+      <c r="F91" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="G91" s="189" t="s">
+      <c r="G91" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="H91" s="186" t="s">
+      <c r="H91" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="I91" s="186" t="s">
+      <c r="I91" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="J91" s="186"/>
-      <c r="K91" s="186" t="s">
+      <c r="J91" s="199"/>
+      <c r="K91" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="L91" s="186" t="s">
+      <c r="L91" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="M91" s="186" t="s">
+      <c r="M91" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="N91" s="186"/>
-      <c r="O91" s="186" t="s">
+      <c r="N91" s="199"/>
+      <c r="O91" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="P91" s="186" t="s">
+      <c r="P91" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="Q91" s="186"/>
+      <c r="Q91" s="199"/>
     </row>
     <row r="92" spans="1:17" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="C92" s="186"/>
-      <c r="D92" s="189"/>
-      <c r="E92" s="186"/>
-      <c r="F92" s="186"/>
-      <c r="G92" s="189"/>
-      <c r="H92" s="186"/>
+      <c r="C92" s="199"/>
+      <c r="D92" s="201"/>
+      <c r="E92" s="199"/>
+      <c r="F92" s="199"/>
+      <c r="G92" s="201"/>
+      <c r="H92" s="199"/>
       <c r="I92" s="24" t="s">
         <v>9</v>
       </c>
       <c r="J92" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K92" s="186"/>
-      <c r="L92" s="186"/>
+      <c r="K92" s="199"/>
+      <c r="L92" s="199"/>
       <c r="M92" s="24" t="s">
         <v>9</v>
       </c>
       <c r="N92" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O92" s="186"/>
-      <c r="P92" s="186"/>
-      <c r="Q92" s="186"/>
+      <c r="O92" s="199"/>
+      <c r="P92" s="199"/>
+      <c r="Q92" s="199"/>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B93" s="4" t="s">
@@ -13486,106 +13317,106 @@
       <c r="B100" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C100" s="195" t="s">
+      <c r="C100" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="D100" s="195"/>
-      <c r="E100" s="195"/>
-      <c r="F100" s="195" t="s">
+      <c r="D100" s="198"/>
+      <c r="E100" s="198"/>
+      <c r="F100" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="G100" s="195"/>
-      <c r="H100" s="195"/>
-      <c r="I100" s="195" t="s">
+      <c r="G100" s="198"/>
+      <c r="H100" s="198"/>
+      <c r="I100" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="J100" s="195"/>
-      <c r="K100" s="195"/>
-      <c r="L100" s="195"/>
-      <c r="M100" s="195" t="s">
+      <c r="J100" s="198"/>
+      <c r="K100" s="198"/>
+      <c r="L100" s="198"/>
+      <c r="M100" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="N100" s="195"/>
-      <c r="O100" s="195"/>
-      <c r="P100" s="195"/>
+      <c r="N100" s="198"/>
+      <c r="O100" s="198"/>
+      <c r="P100" s="198"/>
     </row>
     <row r="101" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C101" s="186" t="s">
+      <c r="C101" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="D101" s="189" t="s">
+      <c r="D101" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="E101" s="186" t="s">
+      <c r="E101" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="F101" s="186" t="s">
+      <c r="F101" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="G101" s="189" t="s">
+      <c r="G101" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="H101" s="186" t="s">
+      <c r="H101" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="I101" s="186" t="s">
+      <c r="I101" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="J101" s="186"/>
-      <c r="K101" s="186" t="s">
+      <c r="J101" s="199"/>
+      <c r="K101" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="L101" s="186" t="s">
+      <c r="L101" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="M101" s="186" t="s">
+      <c r="M101" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="N101" s="186"/>
-      <c r="O101" s="186" t="s">
+      <c r="N101" s="199"/>
+      <c r="O101" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="P101" s="186" t="s">
+      <c r="P101" s="199" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="102" spans="2:16" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="C102" s="186"/>
-      <c r="D102" s="189"/>
-      <c r="E102" s="186"/>
-      <c r="F102" s="186"/>
-      <c r="G102" s="189"/>
-      <c r="H102" s="186"/>
+      <c r="C102" s="199"/>
+      <c r="D102" s="201"/>
+      <c r="E102" s="199"/>
+      <c r="F102" s="199"/>
+      <c r="G102" s="201"/>
+      <c r="H102" s="199"/>
       <c r="I102" s="24" t="s">
         <v>9</v>
       </c>
       <c r="J102" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K102" s="186"/>
-      <c r="L102" s="186"/>
+      <c r="K102" s="199"/>
+      <c r="L102" s="199"/>
       <c r="M102" s="24" t="s">
         <v>9</v>
       </c>
       <c r="N102" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O102" s="186"/>
-      <c r="P102" s="186"/>
+      <c r="O102" s="199"/>
+      <c r="P102" s="199"/>
     </row>
     <row r="103" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B103" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C103" s="200"/>
-      <c r="D103" s="201"/>
-      <c r="E103" s="201"/>
-      <c r="F103" s="200"/>
-      <c r="G103" s="201"/>
-      <c r="H103" s="202"/>
+      <c r="C103" s="186"/>
+      <c r="D103" s="187"/>
+      <c r="E103" s="187"/>
+      <c r="F103" s="186"/>
+      <c r="G103" s="187"/>
+      <c r="H103" s="188"/>
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
       <c r="K103" s="7"/>
@@ -13599,24 +13430,24 @@
       <c r="B104" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C104" s="203"/>
-      <c r="D104" s="204"/>
-      <c r="E104" s="204"/>
-      <c r="F104" s="203"/>
-      <c r="G104" s="204"/>
-      <c r="H104" s="205"/>
+      <c r="C104" s="189"/>
+      <c r="D104" s="190"/>
+      <c r="E104" s="190"/>
+      <c r="F104" s="189"/>
+      <c r="G104" s="190"/>
+      <c r="H104" s="191"/>
       <c r="P104" s="12"/>
     </row>
     <row r="105" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B105" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C105" s="206"/>
-      <c r="D105" s="207"/>
-      <c r="E105" s="207"/>
-      <c r="F105" s="206"/>
-      <c r="G105" s="207"/>
-      <c r="H105" s="208"/>
+      <c r="C105" s="192"/>
+      <c r="D105" s="193"/>
+      <c r="E105" s="193"/>
+      <c r="F105" s="192"/>
+      <c r="G105" s="193"/>
+      <c r="H105" s="194"/>
       <c r="I105" s="52"/>
       <c r="J105" s="52"/>
       <c r="K105" s="52"/>
@@ -13654,106 +13485,106 @@
       <c r="B110" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C110" s="195" t="s">
+      <c r="C110" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="D110" s="195"/>
-      <c r="E110" s="195"/>
-      <c r="F110" s="195" t="s">
+      <c r="D110" s="198"/>
+      <c r="E110" s="198"/>
+      <c r="F110" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="G110" s="195"/>
-      <c r="H110" s="195"/>
-      <c r="I110" s="195" t="s">
+      <c r="G110" s="198"/>
+      <c r="H110" s="198"/>
+      <c r="I110" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="J110" s="195"/>
-      <c r="K110" s="195"/>
-      <c r="L110" s="195"/>
-      <c r="M110" s="195" t="s">
+      <c r="J110" s="198"/>
+      <c r="K110" s="198"/>
+      <c r="L110" s="198"/>
+      <c r="M110" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="N110" s="195"/>
-      <c r="O110" s="195"/>
-      <c r="P110" s="195"/>
+      <c r="N110" s="198"/>
+      <c r="O110" s="198"/>
+      <c r="P110" s="198"/>
     </row>
     <row r="111" spans="2:16" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B111" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C111" s="186" t="s">
+      <c r="C111" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="D111" s="189" t="s">
+      <c r="D111" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="E111" s="186" t="s">
+      <c r="E111" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="F111" s="186" t="s">
+      <c r="F111" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="G111" s="189" t="s">
+      <c r="G111" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="H111" s="186" t="s">
+      <c r="H111" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="I111" s="186" t="s">
+      <c r="I111" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="J111" s="186"/>
-      <c r="K111" s="186" t="s">
+      <c r="J111" s="199"/>
+      <c r="K111" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="L111" s="186" t="s">
+      <c r="L111" s="199" t="s">
         <v>7</v>
       </c>
-      <c r="M111" s="186" t="s">
+      <c r="M111" s="199" t="s">
         <v>5</v>
       </c>
-      <c r="N111" s="186"/>
-      <c r="O111" s="186" t="s">
+      <c r="N111" s="199"/>
+      <c r="O111" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="P111" s="186" t="s">
+      <c r="P111" s="199" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="112" spans="2:16" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="C112" s="186"/>
-      <c r="D112" s="189"/>
-      <c r="E112" s="186"/>
-      <c r="F112" s="186"/>
-      <c r="G112" s="189"/>
-      <c r="H112" s="186"/>
+      <c r="C112" s="199"/>
+      <c r="D112" s="201"/>
+      <c r="E112" s="199"/>
+      <c r="F112" s="199"/>
+      <c r="G112" s="201"/>
+      <c r="H112" s="199"/>
       <c r="I112" s="24" t="s">
         <v>9</v>
       </c>
       <c r="J112" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="K112" s="186"/>
-      <c r="L112" s="186"/>
+      <c r="K112" s="199"/>
+      <c r="L112" s="199"/>
       <c r="M112" s="24" t="s">
         <v>9</v>
       </c>
       <c r="N112" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O112" s="186"/>
-      <c r="P112" s="186"/>
+      <c r="O112" s="199"/>
+      <c r="P112" s="199"/>
     </row>
     <row r="113" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B113" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C113" s="200"/>
-      <c r="D113" s="201"/>
-      <c r="E113" s="201"/>
-      <c r="F113" s="200"/>
-      <c r="G113" s="201"/>
-      <c r="H113" s="202"/>
+      <c r="C113" s="186"/>
+      <c r="D113" s="187"/>
+      <c r="E113" s="187"/>
+      <c r="F113" s="186"/>
+      <c r="G113" s="187"/>
+      <c r="H113" s="188"/>
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
       <c r="K113" s="7"/>
@@ -13767,24 +13598,24 @@
       <c r="B114" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C114" s="203"/>
-      <c r="D114" s="204"/>
-      <c r="E114" s="204"/>
-      <c r="F114" s="203"/>
-      <c r="G114" s="204"/>
-      <c r="H114" s="205"/>
+      <c r="C114" s="189"/>
+      <c r="D114" s="190"/>
+      <c r="E114" s="190"/>
+      <c r="F114" s="189"/>
+      <c r="G114" s="190"/>
+      <c r="H114" s="191"/>
       <c r="P114" s="12"/>
     </row>
     <row r="115" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B115" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C115" s="206"/>
-      <c r="D115" s="207"/>
-      <c r="E115" s="207"/>
-      <c r="F115" s="206"/>
-      <c r="G115" s="207"/>
-      <c r="H115" s="208"/>
+      <c r="C115" s="192"/>
+      <c r="D115" s="193"/>
+      <c r="E115" s="193"/>
+      <c r="F115" s="192"/>
+      <c r="G115" s="193"/>
+      <c r="H115" s="194"/>
       <c r="I115" s="52"/>
       <c r="J115" s="52"/>
       <c r="K115" s="52"/>
@@ -13822,47 +13653,47 @@
       <c r="B120" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C120" s="195" t="s">
+      <c r="C120" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="D120" s="195"/>
-      <c r="E120" s="195"/>
-      <c r="F120" s="195" t="s">
+      <c r="D120" s="198"/>
+      <c r="E120" s="198"/>
+      <c r="F120" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="G120" s="195"/>
-      <c r="H120" s="195"/>
+      <c r="G120" s="198"/>
+      <c r="H120" s="198"/>
     </row>
     <row r="121" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B121" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C121" s="186" t="s">
+      <c r="C121" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="D121" s="189" t="s">
+      <c r="D121" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="E121" s="186" t="s">
+      <c r="E121" s="199" t="s">
         <v>22</v>
       </c>
-      <c r="F121" s="186" t="s">
+      <c r="F121" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="G121" s="189" t="s">
+      <c r="G121" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="H121" s="186" t="s">
+      <c r="H121" s="199" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="122" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C122" s="186"/>
-      <c r="D122" s="189"/>
-      <c r="E122" s="186"/>
-      <c r="F122" s="186"/>
-      <c r="G122" s="189"/>
-      <c r="H122" s="186"/>
+      <c r="C122" s="199"/>
+      <c r="D122" s="201"/>
+      <c r="E122" s="199"/>
+      <c r="F122" s="199"/>
+      <c r="G122" s="201"/>
+      <c r="H122" s="199"/>
     </row>
     <row r="123" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B123" s="4" t="s">
@@ -13970,18 +13801,18 @@
       <c r="H129" s="65"/>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C132" s="195" t="s">
+      <c r="C132" s="198" t="s">
         <v>93</v>
       </c>
-      <c r="D132" s="195"/>
-      <c r="E132" s="195"/>
-      <c r="F132" s="195"/>
-      <c r="G132" s="195" t="s">
+      <c r="D132" s="198"/>
+      <c r="E132" s="198"/>
+      <c r="F132" s="198"/>
+      <c r="G132" s="198" t="s">
         <v>94</v>
       </c>
-      <c r="H132" s="195"/>
-      <c r="I132" s="195"/>
-      <c r="J132" s="195"/>
+      <c r="H132" s="198"/>
+      <c r="I132" s="198"/>
+      <c r="J132" s="198"/>
     </row>
     <row r="133" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C133" s="24" t="s">
@@ -14010,7 +13841,7 @@
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A134" s="199" t="s">
+      <c r="A134" s="211" t="s">
         <v>93</v>
       </c>
       <c r="B134" s="4" t="s">
@@ -14043,7 +13874,7 @@
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A135" s="199"/>
+      <c r="A135" s="211"/>
       <c r="B135" s="4" t="s">
         <v>21</v>
       </c>
@@ -14073,7 +13904,7 @@
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A136" s="199"/>
+      <c r="A136" s="211"/>
       <c r="B136" s="4" t="s">
         <v>22</v>
       </c>
@@ -14103,7 +13934,7 @@
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A137" s="199" t="s">
+      <c r="A137" s="211" t="s">
         <v>94</v>
       </c>
       <c r="B137" s="4" t="s">
@@ -14135,7 +13966,7 @@
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A138" s="199"/>
+      <c r="A138" s="211"/>
       <c r="B138" s="4" t="s">
         <v>21</v>
       </c>
@@ -14165,7 +13996,7 @@
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A139" s="199"/>
+      <c r="A139" s="211"/>
       <c r="B139" s="4" t="s">
         <v>22</v>
       </c>
@@ -14262,120 +14093,6 @@
     </row>
   </sheetData>
   <mergeCells count="138">
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="I25:L25"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="Q26:Q27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="I47:L47"/>
-    <mergeCell ref="M47:P47"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="K48:K49"/>
-    <mergeCell ref="L48:L49"/>
-    <mergeCell ref="M48:N48"/>
-    <mergeCell ref="O48:O49"/>
-    <mergeCell ref="P48:P49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="H68:H69"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="Q90:Q92"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="D91:D92"/>
-    <mergeCell ref="E91:E92"/>
-    <mergeCell ref="P91:P92"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="I90:L90"/>
-    <mergeCell ref="M90:P90"/>
-    <mergeCell ref="M91:N91"/>
-    <mergeCell ref="O91:O92"/>
-    <mergeCell ref="C100:E100"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="D101:D102"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F91:F92"/>
-    <mergeCell ref="G91:G92"/>
-    <mergeCell ref="H91:H92"/>
-    <mergeCell ref="I91:J91"/>
-    <mergeCell ref="K91:K92"/>
-    <mergeCell ref="L91:L92"/>
-    <mergeCell ref="D111:D112"/>
-    <mergeCell ref="E111:E112"/>
-    <mergeCell ref="F111:F112"/>
-    <mergeCell ref="G111:G112"/>
-    <mergeCell ref="H111:H112"/>
-    <mergeCell ref="M100:P100"/>
-    <mergeCell ref="F101:F102"/>
-    <mergeCell ref="G101:G102"/>
-    <mergeCell ref="I101:J101"/>
-    <mergeCell ref="K101:K102"/>
-    <mergeCell ref="L101:L102"/>
-    <mergeCell ref="M101:N101"/>
-    <mergeCell ref="O101:O102"/>
-    <mergeCell ref="P101:P102"/>
-    <mergeCell ref="E101:E102"/>
-    <mergeCell ref="H101:H102"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="I100:L100"/>
     <mergeCell ref="A137:A139"/>
     <mergeCell ref="G132:J132"/>
     <mergeCell ref="A134:A136"/>
@@ -14400,6 +14117,120 @@
     <mergeCell ref="I110:L110"/>
     <mergeCell ref="M110:P110"/>
     <mergeCell ref="C111:C112"/>
+    <mergeCell ref="D111:D112"/>
+    <mergeCell ref="E111:E112"/>
+    <mergeCell ref="F111:F112"/>
+    <mergeCell ref="G111:G112"/>
+    <mergeCell ref="H111:H112"/>
+    <mergeCell ref="M100:P100"/>
+    <mergeCell ref="F101:F102"/>
+    <mergeCell ref="G101:G102"/>
+    <mergeCell ref="I101:J101"/>
+    <mergeCell ref="K101:K102"/>
+    <mergeCell ref="L101:L102"/>
+    <mergeCell ref="M101:N101"/>
+    <mergeCell ref="O101:O102"/>
+    <mergeCell ref="P101:P102"/>
+    <mergeCell ref="E101:E102"/>
+    <mergeCell ref="H101:H102"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="I100:L100"/>
+    <mergeCell ref="C100:E100"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="D101:D102"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F91:F92"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="H91:H92"/>
+    <mergeCell ref="I91:J91"/>
+    <mergeCell ref="K91:K92"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="Q90:Q92"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="D91:D92"/>
+    <mergeCell ref="E91:E92"/>
+    <mergeCell ref="P91:P92"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="I90:L90"/>
+    <mergeCell ref="M90:P90"/>
+    <mergeCell ref="M91:N91"/>
+    <mergeCell ref="O91:O92"/>
+    <mergeCell ref="L91:L92"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="H68:H69"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="K48:K49"/>
+    <mergeCell ref="L48:L49"/>
+    <mergeCell ref="M48:N48"/>
+    <mergeCell ref="O48:O49"/>
+    <mergeCell ref="P48:P49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="Q26:Q27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="I47:L47"/>
+    <mergeCell ref="M47:P47"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>